<commit_message>
Sixth version of the project
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticsInfo.xlsx
+++ b/src/main/resources/statisticsInfo.xlsx
@@ -41,16 +41,16 @@
     <t>Московский Придуманный Институт;Московский Выдуманный Университет;</t>
   </si>
   <si>
+    <t>Лингвистика</t>
+  </si>
+  <si>
+    <t>Воронежский Литературно-Переводческий Университет;</t>
+  </si>
+  <si>
     <t>Математика</t>
   </si>
   <si>
     <t>Казанский Университет Вычислений;</t>
-  </si>
-  <si>
-    <t>Лингвистика</t>
-  </si>
-  <si>
-    <t>Воронежский Литературно-Переводческий Университет;</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Final version of the project
</commit_message>
<xml_diff>
--- a/src/main/resources/statisticsInfo.xlsx
+++ b/src/main/resources/statisticsInfo.xlsx
@@ -29,6 +29,12 @@
     <t>Наименования университетов</t>
   </si>
   <si>
+    <t>Математика</t>
+  </si>
+  <si>
+    <t>Казанский Университет Вычислений;</t>
+  </si>
+  <si>
     <t>Медицина</t>
   </si>
   <si>
@@ -45,12 +51,6 @@
   </si>
   <si>
     <t>Воронежский Литературно-Переводческий Университет;</t>
-  </si>
-  <si>
-    <t>Математика</t>
-  </si>
-  <si>
-    <t>Казанский Университет Вычислений;</t>
   </si>
 </sst>
 </file>
@@ -129,13 +129,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>4.329999923706055</v>
+        <v>0.0</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="E2" t="s" s="0">
         <v>6</v>
@@ -146,13 +146,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>4.539999961853027</v>
+        <v>4.329999923706055</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>8.0</v>
+        <v>3.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E3" t="s" s="0">
         <v>8</v>
@@ -163,13 +163,13 @@
         <v>9</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>0.0</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="E4" t="s" s="0">
         <v>10</v>

</xml_diff>